<commit_message>
new table to compare errors
</commit_message>
<xml_diff>
--- a/summaryVotePredictionModels_holdoutset.xlsx
+++ b/summaryVotePredictionModels_holdoutset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Documents\GitHub\ML_VotingAggregation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8563109B-C58F-4805-A44C-D2E0937094ED}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81DAFE6D-7DAB-4737-AA42-47D59F7875F1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18120" windowHeight="7178" activeTab="4" xr2:uid="{17172B9F-2425-4985-BD43-C4C7130542FC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18120" windowHeight="7178" tabRatio="869" activeTab="10" xr2:uid="{17172B9F-2425-4985-BD43-C4C7130542FC}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="171">
   <si>
     <t>Results from training different ML methods to predict the threshold "n" that indicates if a question covers a fault.</t>
   </si>
@@ -241,9 +241,6 @@
     <t xml:space="preserve">  1.00  1       0.6016007  0.9503526  0.3531785</t>
   </si>
   <si>
-    <t xml:space="preserve">  1.00  2       0.6393799  0.8850063  0.5566535</t>
-  </si>
-  <si>
     <t xml:space="preserve">  1.00  3       0.5632631  0.7458534  0.7327899</t>
   </si>
   <si>
@@ -334,9 +331,6 @@
     <t xml:space="preserve">  1.00  1       0.6077026  0.9285008  0.3737374</t>
   </si>
   <si>
-    <t xml:space="preserve">  1.00  2       0.7655981  0.8735835  0.5768921</t>
-  </si>
-  <si>
     <t xml:space="preserve">  1.00  3       0.6857370  0.8162877  0.6975187</t>
   </si>
   <si>
@@ -455,6 +449,129 @@
   </si>
   <si>
     <t xml:space="preserve">  0.8526932  0.9464095  0.3519598</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>ROC</t>
+  </si>
+  <si>
+    <t>Sensitiviy</t>
+  </si>
+  <si>
+    <t>Specificity</t>
+  </si>
+  <si>
+    <t>Hyper-parameters</t>
+  </si>
+  <si>
+    <t>Validation</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Max threshold</t>
+  </si>
+  <si>
+    <t>Min threshold</t>
+  </si>
+  <si>
+    <t>KNN</t>
+  </si>
+  <si>
+    <t>Random Forest</t>
+  </si>
+  <si>
+    <t>GLM</t>
+  </si>
+  <si>
+    <t>SVM Linear</t>
+  </si>
+  <si>
+    <t>SVM Linear 2</t>
+  </si>
+  <si>
+    <t>SVM Linear Weights</t>
+  </si>
+  <si>
+    <t>Bayes GLM</t>
+  </si>
+  <si>
+    <t>AM.1</t>
+  </si>
+  <si>
+    <t>AM.2</t>
+  </si>
+  <si>
+    <t>AM.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7373141  0.9644698  0.2 </t>
+  </si>
+  <si>
+    <t>0.7862716  0.9731959  0.1272727</t>
+  </si>
+  <si>
+    <t>0.7538838  0.955102  0.2272727</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6016007  0.9503526  0.3531785</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6093731  0.9690839  0.1559069</t>
+  </si>
+  <si>
+    <t>0.7673846  0.9285008  0.3737374</t>
+  </si>
+  <si>
+    <t>Final values for the model cost = 1 and weight = 2</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  1.00  2     </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">  0.6393799  0.8850063  0.5566535</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.6393799  0.8850063  0.5566535</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6886753  0.8696407  0.5791063</t>
+  </si>
+  <si>
+    <t>Final values for the model cost = 1 and weight = 2.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  1.00  2      </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> 0.7655981  0.8735835  0.5768921</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.7655981  0.8735835  0.5768921</t>
   </si>
 </sst>
 </file>
@@ -491,7 +608,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -501,6 +618,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -597,7 +726,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -645,11 +774,32 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -660,6 +810,57 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A2CB4001-E8C7-44CA-A9BB-A5E9467F6052}" name="Table1" displayName="Table1" ref="B3:I11" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="B3:I11" xr:uid="{779F2AB1-492F-4A3F-8764-B23C6934AA38}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{9C741884-A7A5-4507-B313-29474FBBAE2D}" name="Model"/>
+    <tableColumn id="2" xr3:uid="{02581FDB-E7BF-4CDD-A717-B60C9A2056CA}" name="Hyper-parameters"/>
+    <tableColumn id="3" xr3:uid="{96D452D4-358F-4FE2-935F-3C28D10FC3ED}" name="ROC"/>
+    <tableColumn id="4" xr3:uid="{02E4A108-7BC5-430F-9E56-61AA251E2FD4}" name="Sensitiviy"/>
+    <tableColumn id="5" xr3:uid="{455737C9-8EBD-4CAD-BC06-293290ACBFF0}" name="Specificity"/>
+    <tableColumn id="6" xr3:uid="{ED4572A9-08A3-4B04-AF59-4464029ADBC0}" name="Error"/>
+    <tableColumn id="7" xr3:uid="{BC4BD792-E741-4BBB-A371-C4436F6CD771}" name="Max threshold"/>
+    <tableColumn id="8" xr3:uid="{8702C136-6D5F-4282-B862-2F623B877E2C}" name="Min threshold"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E5D5859A-64DA-4306-8EFE-9DE35FA7BA3C}" name="Table13" displayName="Table13" ref="B15:I23" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="B15:I23" xr:uid="{0FA4A9D6-D37E-41B6-9DCB-04BC8626433A}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{5DF7AFE4-C157-4605-B717-10D1B7151790}" name="Model"/>
+    <tableColumn id="2" xr3:uid="{CF0875DB-C216-4008-9DBB-3C6322318C8D}" name="Hyper-parameters"/>
+    <tableColumn id="3" xr3:uid="{FBABBDEC-099B-4E5D-A924-A62971F87DBD}" name="ROC"/>
+    <tableColumn id="4" xr3:uid="{E06E8967-0EB2-4487-8F07-41D2872B931E}" name="Sensitiviy"/>
+    <tableColumn id="5" xr3:uid="{E9623A23-A9D3-4D98-BA5B-050C960B7B0D}" name="Specificity"/>
+    <tableColumn id="6" xr3:uid="{4CA7ECC5-B446-4520-AB93-CAB392EC600F}" name="Error"/>
+    <tableColumn id="7" xr3:uid="{940E105C-0866-4E83-9B2B-C0350F4B4108}" name="Max threshold"/>
+    <tableColumn id="8" xr3:uid="{0C5E143F-E1A4-4DF9-87CC-794A29B8691A}" name="Min threshold"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FEA6ED00-372F-473E-86A7-A1FAD000CD94}" name="Table134" displayName="Table134" ref="B26:I34" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="B26:I34" xr:uid="{4071A98A-9B8F-454F-98CA-3B3B96010D64}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{15F49AF9-4268-479A-AE3E-663E847DFF19}" name="Model"/>
+    <tableColumn id="2" xr3:uid="{462B6A13-580B-4B95-8465-99A5F46CBBEE}" name="Hyper-parameters"/>
+    <tableColumn id="3" xr3:uid="{C60D4BF0-8167-4494-8374-A803A3EB4AD8}" name="ROC"/>
+    <tableColumn id="4" xr3:uid="{9233DEE9-F594-4F97-A407-E387D3F18D28}" name="Sensitiviy"/>
+    <tableColumn id="5" xr3:uid="{5272C310-BB30-4DC0-B063-5B4283F689DA}" name="Specificity"/>
+    <tableColumn id="6" xr3:uid="{3F7FA1FB-F76D-4296-9BEA-DD1F87E32325}" name="Error"/>
+    <tableColumn id="7" xr3:uid="{1BF3C9D3-92D2-4968-8174-865F158AB08F}" name="Max threshold"/>
+    <tableColumn id="8" xr3:uid="{FB912703-7541-4ECF-A019-68CCCDE49511}" name="Min threshold"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -962,7 +1163,7 @@
   <dimension ref="B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -981,8 +1182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A75EDD9-FA8A-4EAA-BA64-88C298486E2C}">
   <dimension ref="B1:U20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1057,7 +1258,7 @@
       <c r="F6" s="10"/>
       <c r="G6" s="11"/>
       <c r="I6" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
@@ -1065,7 +1266,7 @@
       <c r="M6" s="10"/>
       <c r="N6" s="11"/>
       <c r="P6" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q6" s="10"/>
       <c r="R6" s="10"/>
@@ -1155,7 +1356,7 @@
       <c r="F10" s="10"/>
       <c r="G10" s="11"/>
       <c r="I10" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
@@ -1163,7 +1364,7 @@
       <c r="M10" s="10"/>
       <c r="N10" s="11"/>
       <c r="P10" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q10" s="10"/>
       <c r="R10" s="10"/>
@@ -1181,7 +1382,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="11"/>
       <c r="I11" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J11" s="14"/>
       <c r="K11" s="14"/>
@@ -1189,7 +1390,7 @@
       <c r="M11" s="14"/>
       <c r="N11" s="15"/>
       <c r="P11" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q11" s="14"/>
       <c r="R11" s="14"/>
@@ -1207,10 +1408,10 @@
       <c r="F12" s="14"/>
       <c r="G12" s="15"/>
       <c r="I12" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.45">
@@ -1218,10 +1419,10 @@
         <v>64</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.45">
@@ -1229,10 +1430,10 @@
         <v>65</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.45">
@@ -1240,10 +1441,10 @@
         <v>66</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.45">
@@ -1251,29 +1452,29 @@
         <v>67</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B17" s="2" t="s">
-        <v>68</v>
+        <v>165</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>99</v>
+        <v>169</v>
       </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B18" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>118</v>
+        <v>68</v>
+      </c>
+      <c r="I18" s="29" t="s">
+        <v>116</v>
       </c>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
@@ -1281,18 +1482,18 @@
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="P18" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B20" s="2" t="s">
-        <v>102</v>
+        <v>164</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>102</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -1302,13 +1503,364 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C55AC194-8843-4B46-935F-A3DF9CFDC7A7}">
-  <dimension ref="A1"/>
+  <dimension ref="B2:I34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="17.9296875" customWidth="1"/>
+    <col min="3" max="3" width="17.3984375" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="9" max="9" width="14.1328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B2" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="I3" s="23" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>0.5860649</v>
+      </c>
+      <c r="E4">
+        <v>0.85667219999999999</v>
+      </c>
+      <c r="F4">
+        <v>0.51589739999999995</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B6" t="s">
+        <v>149</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B7" t="s">
+        <v>150</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B9" t="s">
+        <v>151</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B10" t="s">
+        <v>152</v>
+      </c>
+      <c r="D10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
+        <v>153</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B14" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B15" t="s">
+        <v>138</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="H15" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="I15" s="23" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16">
+        <v>0.63291260000000005</v>
+      </c>
+      <c r="E16">
+        <v>0.90811969999999997</v>
+      </c>
+      <c r="F16">
+        <v>0.42460320000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B17" t="s">
+        <v>148</v>
+      </c>
+      <c r="D17" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B18" t="s">
+        <v>149</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B19" t="s">
+        <v>150</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B20" t="s">
+        <v>154</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B21" t="s">
+        <v>151</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B22" t="s">
+        <v>152</v>
+      </c>
+      <c r="D22" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B23" t="s">
+        <v>153</v>
+      </c>
+      <c r="D23" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B25" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="H25" s="25"/>
+      <c r="I25" s="25"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B26" t="s">
+        <v>138</v>
+      </c>
+      <c r="C26" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="D26" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="E26" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="G26" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="H26" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="I26" s="23" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27">
+        <v>0.63323660000000004</v>
+      </c>
+      <c r="E27">
+        <v>0.89907970000000004</v>
+      </c>
+      <c r="F27">
+        <v>0.56031750000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B28" t="s">
+        <v>148</v>
+      </c>
+      <c r="D28" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B29" t="s">
+        <v>149</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B30" t="s">
+        <v>150</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B31" t="s">
+        <v>154</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B32" t="s">
+        <v>151</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B33" t="s">
+        <v>152</v>
+      </c>
+      <c r="D33" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B34" t="s">
+        <v>153</v>
+      </c>
+      <c r="D34" t="s">
+        <v>170</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="3">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1317,7 +1869,7 @@
   <dimension ref="B1:N20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1381,7 +1933,7 @@
       <c r="F6" s="10"/>
       <c r="G6" s="11"/>
       <c r="I6" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
@@ -1449,7 +2001,7 @@
       <c r="F10" s="10"/>
       <c r="G10" s="11"/>
       <c r="I10" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
@@ -1467,7 +2019,7 @@
       <c r="F11" s="14"/>
       <c r="G11" s="15"/>
       <c r="I11" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J11" s="14"/>
       <c r="K11" s="14"/>
@@ -1486,7 +2038,7 @@
       <c r="F14" s="7"/>
       <c r="G14" s="8"/>
       <c r="I14" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.45">
@@ -1499,7 +2051,7 @@
       <c r="F15" s="10"/>
       <c r="G15" s="11"/>
       <c r="I15" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.45">
@@ -1523,7 +2075,7 @@
       <c r="F17" s="10"/>
       <c r="G17" s="11"/>
       <c r="I17" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.45">
@@ -1567,7 +2119,7 @@
   <dimension ref="B1:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1637,7 +2189,7 @@
       <c r="F6" s="10"/>
       <c r="G6" s="11"/>
       <c r="I6" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
@@ -1682,7 +2234,7 @@
       <c r="F9" s="10"/>
       <c r="G9" s="11"/>
       <c r="I9" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
@@ -1700,7 +2252,7 @@
       <c r="F10" s="10"/>
       <c r="G10" s="11"/>
       <c r="I10" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J10" s="22"/>
       <c r="K10" s="22"/>
@@ -1718,7 +2270,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="15"/>
       <c r="I11" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="J11" s="14"/>
       <c r="K11" s="14"/>
@@ -1735,7 +2287,7 @@
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
       <c r="I12" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
@@ -1751,7 +2303,7 @@
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B15" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
@@ -1779,7 +2331,7 @@
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B18" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
@@ -1789,7 +2341,7 @@
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B19" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C19" s="22"/>
       <c r="D19" s="22"/>
@@ -1799,7 +2351,7 @@
     </row>
     <row r="20" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B20" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C20" s="14"/>
       <c r="D20" s="14"/>
@@ -1809,7 +2361,7 @@
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B21" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1823,7 +2375,7 @@
   <dimension ref="B1:N20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1888,7 +2440,7 @@
       <c r="F6" s="10"/>
       <c r="G6" s="11"/>
       <c r="I6" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
@@ -1952,7 +2504,7 @@
       <c r="F10" s="10"/>
       <c r="G10" s="11"/>
       <c r="I10" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
@@ -1987,7 +2539,7 @@
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B15" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
@@ -2028,7 +2580,7 @@
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B19" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
@@ -2054,8 +2606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBD8369C-2B36-4B2D-B1CD-E8847EE64B5F}">
   <dimension ref="B1:U23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2142,7 +2694,7 @@
       <c r="M6" s="10"/>
       <c r="N6" s="11"/>
       <c r="P6" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q6" s="10"/>
       <c r="R6" s="10"/>
@@ -2192,7 +2744,7 @@
       <c r="F9" s="10"/>
       <c r="G9" s="11"/>
       <c r="I9" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
@@ -2200,7 +2752,7 @@
       <c r="M9" s="10"/>
       <c r="N9" s="11"/>
       <c r="P9" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q9" s="10"/>
       <c r="R9" s="10"/>
@@ -2209,7 +2761,7 @@
       <c r="U9" s="11"/>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.45">
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="21" t="s">
         <v>33</v>
       </c>
       <c r="C10" s="10"/>
@@ -2217,16 +2769,16 @@
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
       <c r="G10" s="11"/>
-      <c r="I10" s="2" t="s">
-        <v>129</v>
+      <c r="I10" s="5" t="s">
+        <v>127</v>
       </c>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
       <c r="N10" s="11"/>
-      <c r="P10" s="2" t="s">
-        <v>77</v>
+      <c r="P10" s="5" t="s">
+        <v>76</v>
       </c>
       <c r="Q10" s="10"/>
       <c r="R10" s="10"/>
@@ -2244,7 +2796,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="11"/>
       <c r="I11" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
@@ -2252,7 +2804,7 @@
       <c r="M11" s="10"/>
       <c r="N11" s="11"/>
       <c r="P11" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Q11" s="14"/>
       <c r="R11" s="14"/>
@@ -2270,7 +2822,7 @@
       <c r="F12" s="10"/>
       <c r="G12" s="11"/>
       <c r="I12" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J12" s="14"/>
       <c r="K12" s="14"/>
@@ -2278,7 +2830,7 @@
       <c r="M12" s="14"/>
       <c r="N12" s="15"/>
       <c r="P12" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.45">
@@ -2291,10 +2843,10 @@
       <c r="F13" s="10"/>
       <c r="G13" s="11"/>
       <c r="I13" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.45">
@@ -2307,10 +2859,10 @@
       <c r="F14" s="10"/>
       <c r="G14" s="11"/>
       <c r="I14" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.45">
@@ -2323,10 +2875,10 @@
       <c r="F15" s="10"/>
       <c r="G15" s="11"/>
       <c r="I15" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.45">
@@ -2339,10 +2891,10 @@
       <c r="F16" s="10"/>
       <c r="G16" s="11"/>
       <c r="I16" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.45">
@@ -2355,10 +2907,10 @@
       <c r="F17" s="10"/>
       <c r="G17" s="11"/>
       <c r="I17" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -2371,10 +2923,10 @@
       <c r="F18" s="14"/>
       <c r="G18" s="15"/>
       <c r="I18" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="P18" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.45">
@@ -2408,7 +2960,7 @@
   <dimension ref="B1:N20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2474,7 +3026,7 @@
       <c r="F6" s="10"/>
       <c r="G6" s="11"/>
       <c r="I6" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
@@ -2542,7 +3094,7 @@
       <c r="F10" s="10"/>
       <c r="G10" s="11"/>
       <c r="I10" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
@@ -2577,7 +3129,7 @@
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B15" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
@@ -2615,7 +3167,7 @@
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B19" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
@@ -2642,7 +3194,7 @@
   <dimension ref="B1:N20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2708,7 +3260,7 @@
       <c r="F6" s="10"/>
       <c r="G6" s="11"/>
       <c r="I6" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
@@ -2776,7 +3328,7 @@
       <c r="F10" s="10"/>
       <c r="G10" s="11"/>
       <c r="I10" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
@@ -2811,7 +3363,7 @@
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B15" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
@@ -2849,7 +3401,7 @@
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B19" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
@@ -2875,7 +3427,7 @@
   <dimension ref="B1:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2943,7 +3495,7 @@
       <c r="F6" s="10"/>
       <c r="G6" s="11"/>
       <c r="I6" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
@@ -2993,7 +3545,7 @@
       <c r="F9" s="10"/>
       <c r="G9" s="11"/>
       <c r="I9" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
@@ -3011,7 +3563,7 @@
       <c r="F10" s="10"/>
       <c r="G10" s="11"/>
       <c r="I10" s="18" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
@@ -3054,7 +3606,7 @@
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B15" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
@@ -3092,7 +3644,7 @@
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B19" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
@@ -3122,8 +3674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7343E12-5BB3-4E05-86A3-820D943E7119}">
   <dimension ref="B1:N22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3193,7 +3745,7 @@
       <c r="F6" s="10"/>
       <c r="G6" s="11"/>
       <c r="I6" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
@@ -3260,8 +3812,8 @@
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
       <c r="G10" s="11"/>
-      <c r="I10" s="2" t="s">
-        <v>104</v>
+      <c r="I10" s="5" t="s">
+        <v>102</v>
       </c>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
@@ -3279,7 +3831,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="11"/>
       <c r="I11" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J11" s="14"/>
       <c r="K11" s="14"/>
@@ -3297,15 +3849,15 @@
       <c r="F12" s="20"/>
       <c r="G12" s="15"/>
       <c r="I12" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B13" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
@@ -3321,7 +3873,7 @@
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B16" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
@@ -3359,7 +3911,7 @@
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B20" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
@@ -3369,7 +3921,7 @@
     </row>
     <row r="21" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B21" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C21" s="14"/>
       <c r="D21" s="14"/>
@@ -3378,8 +3930,8 @@
       <c r="G21" s="15"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B22" s="3" t="s">
-        <v>91</v>
+      <c r="B22" s="29" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>